<commit_message>
Added new order form
</commit_message>
<xml_diff>
--- a/17ELD002 Product Order Form.xlsx
+++ b/17ELD002 Product Order Form.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18827"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Themb\Documents\GroupProjectDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Themb\Documents\G-ProjectDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t xml:space="preserve"> PURCHASE ORDER REQUEST FORM</t>
   </si>
@@ -132,16 +132,22 @@
     <t>Version March 2011</t>
   </si>
   <si>
-    <t>B06XKMZ3T9</t>
-  </si>
-  <si>
     <t>Themba Kaonga</t>
   </si>
   <si>
     <t>t.m.t.kaonga-14@student.lboro.ac.uk</t>
   </si>
   <si>
-    <t>B018Y127LG</t>
+    <t>B00YOSA85Q</t>
+  </si>
+  <si>
+    <t>B00NH12O5I</t>
+  </si>
+  <si>
+    <t>B00Z05JMKO</t>
+  </si>
+  <si>
+    <t>T.K</t>
   </si>
 </sst>
 </file>
@@ -152,7 +158,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -230,6 +236,24 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1001,7 +1025,7 @@
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1102,10 +1126,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="44" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1168,9 +1188,122 @@
     <xf numFmtId="44" fontId="7" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="55" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1180,63 +1313,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="33" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1309,6 +1385,60 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="33" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1318,122 +1448,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="55" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1512,21 +1531,28 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" tIns="0" bIns="0" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPts val="1500"/>
-            </a:lnSpc>
-          </a:pPr>
           <a:r>
             <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>Elegoo MEGA </a:t>
+            <a:t>HDMI to DVI Cable</a:t>
           </a:r>
           <a:br>
             <a:rPr lang="en-GB" sz="1100"/>
           </a:br>
           <a:r>
-            <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>Genuino Uno </a:t>
+            <a:rPr lang="en-GB"/>
+            <a:t>AmazonBasics</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1050" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> USB 3.0 Male-Female Extension Cable 3m </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1535,7 +1561,10 @@
               <a:spcPts val="1500"/>
             </a:lnSpc>
           </a:pPr>
-          <a:endParaRPr lang="en-GB" sz="1100"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>DisplayPort to HDMI Cable</a:t>
+          </a:r>
         </a:p>
         <a:p>
           <a:pPr>
@@ -1917,7 +1946,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>Geronimoooo</a:t>
+            <a:t>Amazon</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1932,15 +1961,72 @@
           <a:endParaRPr lang="en-GB" sz="1100"/>
         </a:p>
         <a:p>
-          <a:pPr>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
             <a:lnSpc>
               <a:spcPts val="1500"/>
             </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-GB" sz="1100"/>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>amazon.co.uk</a:t>
           </a:r>
+          <a:endParaRPr lang="en-GB">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPts val="1500"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>amazon.co.uk</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -2280,8 +2366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45:H45"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="96" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.5" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2328,122 +2414,122 @@
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="109" t="s">
+      <c r="A5" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="110"/>
-      <c r="C5" s="110"/>
-      <c r="D5" s="110"/>
-      <c r="E5" s="110"/>
-      <c r="F5" s="110"/>
-      <c r="G5" s="110"/>
-      <c r="H5" s="111"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="53"/>
     </row>
     <row r="6" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="112" t="s">
+      <c r="A6" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="113"/>
-      <c r="C6" s="113"/>
-      <c r="D6" s="113"/>
-      <c r="E6" s="113"/>
-      <c r="F6" s="113"/>
-      <c r="G6" s="113"/>
-      <c r="H6" s="114"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="56"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="25"/>
-      <c r="C7" s="123"/>
-      <c r="D7" s="124"/>
-      <c r="E7" s="124"/>
-      <c r="F7" s="124"/>
-      <c r="G7" s="124"/>
-      <c r="H7" s="125"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="69"/>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="27"/>
-      <c r="C8" s="126"/>
-      <c r="D8" s="127"/>
-      <c r="E8" s="127"/>
-      <c r="F8" s="127"/>
-      <c r="G8" s="127"/>
-      <c r="H8" s="128"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="72"/>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="118" t="s">
+      <c r="A9" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="119"/>
-      <c r="C9" s="129"/>
-      <c r="D9" s="130"/>
-      <c r="E9" s="130"/>
-      <c r="F9" s="130"/>
-      <c r="G9" s="130"/>
-      <c r="H9" s="131"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="75"/>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="28"/>
       <c r="B10" s="29"/>
-      <c r="C10" s="126"/>
-      <c r="D10" s="127"/>
-      <c r="E10" s="127"/>
-      <c r="F10" s="127"/>
-      <c r="G10" s="127"/>
-      <c r="H10" s="128"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="72"/>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="135" t="s">
+      <c r="A11" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="136"/>
-      <c r="C11" s="126"/>
-      <c r="D11" s="127"/>
-      <c r="E11" s="127"/>
-      <c r="F11" s="127"/>
-      <c r="G11" s="127"/>
-      <c r="H11" s="128"/>
+      <c r="B11" s="80"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="71"/>
+      <c r="H11" s="72"/>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="135" t="s">
+      <c r="A12" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="136"/>
-      <c r="C12" s="126"/>
-      <c r="D12" s="127"/>
-      <c r="E12" s="127"/>
-      <c r="F12" s="127"/>
-      <c r="G12" s="127"/>
-      <c r="H12" s="128"/>
+      <c r="B12" s="80"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="72"/>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="98" t="s">
+      <c r="A13" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="99"/>
-      <c r="C13" s="132"/>
-      <c r="D13" s="133"/>
-      <c r="E13" s="133"/>
-      <c r="F13" s="133"/>
-      <c r="G13" s="133"/>
-      <c r="H13" s="134"/>
+      <c r="B13" s="66"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="77"/>
+      <c r="E13" s="77"/>
+      <c r="F13" s="77"/>
+      <c r="G13" s="77"/>
+      <c r="H13" s="78"/>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="98" t="s">
+      <c r="A14" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="99"/>
-      <c r="C14" s="132"/>
-      <c r="D14" s="133"/>
-      <c r="E14" s="133"/>
-      <c r="F14" s="133"/>
-      <c r="G14" s="133"/>
-      <c r="H14" s="134"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="77"/>
+      <c r="E14" s="77"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="77"/>
+      <c r="H14" s="78"/>
     </row>
     <row r="15" spans="1:8" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="22"/>
@@ -2452,32 +2538,32 @@
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="74" t="s">
+      <c r="G15" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="H15" s="75"/>
+      <c r="H15" s="94"/>
     </row>
     <row r="16" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="100" t="s">
+      <c r="A16" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="101"/>
-      <c r="C16" s="101"/>
-      <c r="D16" s="101"/>
-      <c r="E16" s="101"/>
-      <c r="F16" s="120" t="s">
+      <c r="B16" s="89"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="89"/>
+      <c r="E16" s="89"/>
+      <c r="F16" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="G16" s="121"/>
-      <c r="H16" s="122"/>
+      <c r="G16" s="63"/>
+      <c r="H16" s="64"/>
     </row>
     <row r="17" spans="1:8" s="19" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="115" t="s">
+      <c r="A17" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="116"/>
-      <c r="C17" s="116"/>
-      <c r="D17" s="117"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="59"/>
       <c r="E17" s="17" t="s">
         <v>2</v>
       </c>
@@ -2492,282 +2578,288 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="92"/>
-      <c r="B18" s="93"/>
-      <c r="C18" s="93"/>
-      <c r="D18" s="94"/>
+      <c r="A18" s="111"/>
+      <c r="B18" s="112"/>
+      <c r="C18" s="112"/>
+      <c r="D18" s="113"/>
       <c r="E18" s="5"/>
       <c r="F18" s="4"/>
       <c r="G18" s="5"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="89"/>
-      <c r="B19" s="90"/>
-      <c r="C19" s="90"/>
-      <c r="D19" s="91"/>
-      <c r="E19" s="52" t="s">
-        <v>36</v>
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="108"/>
+      <c r="B19" s="109"/>
+      <c r="C19" s="109"/>
+      <c r="D19" s="110"/>
+      <c r="E19" s="135" t="s">
+        <v>38</v>
       </c>
       <c r="F19" s="30">
+        <v>2</v>
+      </c>
+      <c r="G19" s="31">
+        <v>5.49</v>
+      </c>
+      <c r="H19" s="48">
+        <f>IF(G19="","",G19*F19)</f>
+        <v>10.98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="90"/>
+      <c r="B20" s="91"/>
+      <c r="C20" s="91"/>
+      <c r="D20" s="92"/>
+      <c r="E20" s="134" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="30">
+        <v>2</v>
+      </c>
+      <c r="G20" s="31">
+        <v>6.49</v>
+      </c>
+      <c r="H20" s="48">
+        <f t="shared" ref="H20:H37" si="0">IF(G20="","",G20*F20)</f>
+        <v>12.98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="90"/>
+      <c r="B21" s="91"/>
+      <c r="C21" s="91"/>
+      <c r="D21" s="92"/>
+      <c r="E21" s="136" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="30">
         <v>1</v>
       </c>
-      <c r="G19" s="31">
-        <v>11.99</v>
-      </c>
-      <c r="H19" s="49">
-        <f>IF(G19="","",G19*F19)</f>
-        <v>11.99</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="53"/>
-      <c r="B20" s="54"/>
-      <c r="C20" s="54"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="52" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20" s="30">
-        <v>1</v>
-      </c>
-      <c r="G20" s="31">
-        <v>22</v>
-      </c>
-      <c r="H20" s="49">
-        <f t="shared" ref="H20:H37" si="0">IF(G20="","",G20*F20)</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="53"/>
-      <c r="B21" s="54"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="50" t="str">
+      <c r="G21" s="33">
+        <v>5.99</v>
+      </c>
+      <c r="H21" s="49">
         <f>IF(G21="","",G21*F21)</f>
-        <v/>
+        <v>5.99</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="53"/>
-      <c r="B22" s="54"/>
-      <c r="C22" s="54"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="32"/>
+      <c r="A22" s="90"/>
+      <c r="B22" s="91"/>
+      <c r="C22" s="91"/>
+      <c r="D22" s="92"/>
+      <c r="E22" s="134"/>
       <c r="F22" s="30"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="50" t="str">
+      <c r="G22" s="33"/>
+      <c r="H22" s="49" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="53"/>
-      <c r="B23" s="54"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="55"/>
+      <c r="A23" s="90"/>
+      <c r="B23" s="91"/>
+      <c r="C23" s="91"/>
+      <c r="D23" s="92"/>
       <c r="E23" s="32"/>
       <c r="F23" s="30"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="50" t="str">
+      <c r="G23" s="33"/>
+      <c r="H23" s="49" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="53"/>
-      <c r="B24" s="54"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="55"/>
+      <c r="A24" s="90"/>
+      <c r="B24" s="91"/>
+      <c r="C24" s="91"/>
+      <c r="D24" s="92"/>
       <c r="E24" s="32"/>
       <c r="F24" s="30"/>
       <c r="G24" s="31"/>
-      <c r="H24" s="50" t="str">
+      <c r="H24" s="49" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="53"/>
-      <c r="B25" s="54"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="55"/>
+      <c r="A25" s="90"/>
+      <c r="B25" s="91"/>
+      <c r="C25" s="91"/>
+      <c r="D25" s="92"/>
       <c r="E25" s="32"/>
       <c r="F25" s="30"/>
       <c r="G25" s="31"/>
-      <c r="H25" s="50" t="str">
+      <c r="H25" s="49" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="53"/>
-      <c r="B26" s="54"/>
-      <c r="C26" s="54"/>
-      <c r="D26" s="55"/>
+      <c r="A26" s="90"/>
+      <c r="B26" s="91"/>
+      <c r="C26" s="91"/>
+      <c r="D26" s="92"/>
       <c r="E26" s="32"/>
       <c r="F26" s="30"/>
       <c r="G26" s="31"/>
-      <c r="H26" s="50" t="str">
+      <c r="H26" s="49" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="53"/>
-      <c r="B27" s="54"/>
-      <c r="C27" s="54"/>
-      <c r="D27" s="55"/>
+      <c r="A27" s="90"/>
+      <c r="B27" s="91"/>
+      <c r="C27" s="91"/>
+      <c r="D27" s="92"/>
       <c r="E27" s="32"/>
       <c r="F27" s="30"/>
       <c r="G27" s="31"/>
-      <c r="H27" s="50" t="str">
+      <c r="H27" s="49" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="53"/>
-      <c r="B28" s="54"/>
-      <c r="C28" s="54"/>
-      <c r="D28" s="55"/>
+      <c r="A28" s="90"/>
+      <c r="B28" s="91"/>
+      <c r="C28" s="91"/>
+      <c r="D28" s="92"/>
       <c r="E28" s="32"/>
       <c r="F28" s="30"/>
       <c r="G28" s="31"/>
-      <c r="H28" s="50" t="str">
+      <c r="H28" s="49" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="53"/>
-      <c r="B29" s="54"/>
-      <c r="C29" s="54"/>
-      <c r="D29" s="55"/>
+      <c r="A29" s="90"/>
+      <c r="B29" s="91"/>
+      <c r="C29" s="91"/>
+      <c r="D29" s="92"/>
       <c r="E29" s="32"/>
       <c r="F29" s="30"/>
       <c r="G29" s="31"/>
-      <c r="H29" s="50" t="str">
+      <c r="H29" s="49" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="53"/>
-      <c r="B30" s="54"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="55"/>
+      <c r="A30" s="90"/>
+      <c r="B30" s="91"/>
+      <c r="C30" s="91"/>
+      <c r="D30" s="92"/>
       <c r="E30" s="32"/>
       <c r="F30" s="30"/>
       <c r="G30" s="31"/>
-      <c r="H30" s="50" t="str">
+      <c r="H30" s="49" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="53"/>
-      <c r="B31" s="54"/>
-      <c r="C31" s="54"/>
-      <c r="D31" s="55"/>
+      <c r="A31" s="90"/>
+      <c r="B31" s="91"/>
+      <c r="C31" s="91"/>
+      <c r="D31" s="92"/>
       <c r="E31" s="32"/>
       <c r="F31" s="30"/>
       <c r="G31" s="31"/>
-      <c r="H31" s="50" t="str">
+      <c r="H31" s="49" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="53"/>
-      <c r="B32" s="54"/>
-      <c r="C32" s="54"/>
-      <c r="D32" s="55"/>
+      <c r="A32" s="90"/>
+      <c r="B32" s="91"/>
+      <c r="C32" s="91"/>
+      <c r="D32" s="92"/>
       <c r="E32" s="32"/>
       <c r="F32" s="30"/>
       <c r="G32" s="31"/>
-      <c r="H32" s="50" t="str">
+      <c r="H32" s="49" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="53"/>
-      <c r="B33" s="54"/>
-      <c r="C33" s="54"/>
-      <c r="D33" s="55"/>
+      <c r="A33" s="90"/>
+      <c r="B33" s="91"/>
+      <c r="C33" s="91"/>
+      <c r="D33" s="92"/>
       <c r="E33" s="32"/>
       <c r="F33" s="30"/>
       <c r="G33" s="31"/>
-      <c r="H33" s="50" t="str">
+      <c r="H33" s="49" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="53"/>
-      <c r="B34" s="54"/>
-      <c r="C34" s="54"/>
-      <c r="D34" s="55"/>
+      <c r="A34" s="90"/>
+      <c r="B34" s="91"/>
+      <c r="C34" s="91"/>
+      <c r="D34" s="92"/>
       <c r="E34" s="32"/>
       <c r="F34" s="30"/>
       <c r="G34" s="31"/>
-      <c r="H34" s="50" t="str">
+      <c r="H34" s="49" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="53"/>
-      <c r="B35" s="54"/>
-      <c r="C35" s="54"/>
-      <c r="D35" s="55"/>
+      <c r="A35" s="90"/>
+      <c r="B35" s="91"/>
+      <c r="C35" s="91"/>
+      <c r="D35" s="92"/>
       <c r="E35" s="32"/>
       <c r="F35" s="30"/>
       <c r="G35" s="31"/>
-      <c r="H35" s="50" t="str">
+      <c r="H35" s="49" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="53"/>
-      <c r="B36" s="54"/>
-      <c r="C36" s="54"/>
-      <c r="D36" s="55"/>
+      <c r="A36" s="90"/>
+      <c r="B36" s="91"/>
+      <c r="C36" s="91"/>
+      <c r="D36" s="92"/>
       <c r="E36" s="32"/>
       <c r="F36" s="30"/>
       <c r="G36" s="31"/>
-      <c r="H36" s="50"/>
+      <c r="H36" s="49"/>
     </row>
     <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="84"/>
-      <c r="B37" s="85"/>
-      <c r="C37" s="85"/>
-      <c r="D37" s="86"/>
-      <c r="E37" s="35"/>
+      <c r="A37" s="103"/>
+      <c r="B37" s="104"/>
+      <c r="C37" s="104"/>
+      <c r="D37" s="105"/>
+      <c r="E37" s="34"/>
       <c r="F37" s="30"/>
       <c r="G37" s="31"/>
-      <c r="H37" s="49" t="str">
+      <c r="H37" s="48" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="38" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="95" t="s">
+      <c r="A38" s="131" t="s">
         <v>22</v>
       </c>
-      <c r="B38" s="96"/>
-      <c r="C38" s="96"/>
-      <c r="D38" s="96"/>
-      <c r="E38" s="97"/>
+      <c r="B38" s="132"/>
+      <c r="C38" s="132"/>
+      <c r="D38" s="132"/>
+      <c r="E38" s="133"/>
       <c r="F38" s="7"/>
       <c r="G38" s="8"/>
-      <c r="H38" s="51"/>
+      <c r="H38" s="50"/>
     </row>
     <row r="39" spans="1:8" s="20" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
@@ -2776,203 +2868,205 @@
       <c r="B39" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C39" s="87" t="s">
+      <c r="C39" s="106" t="s">
         <v>7</v>
       </c>
-      <c r="D39" s="88"/>
-      <c r="E39" s="87" t="s">
+      <c r="D39" s="107"/>
+      <c r="E39" s="106" t="s">
         <v>8</v>
       </c>
-      <c r="F39" s="88"/>
+      <c r="F39" s="107"/>
       <c r="G39" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H39" s="41"/>
+      <c r="H39" s="40"/>
     </row>
     <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="36"/>
-      <c r="B40" s="39"/>
-      <c r="C40" s="78">
+      <c r="A40" s="35"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="97">
         <f>H43</f>
-        <v>40.79</v>
-      </c>
-      <c r="D40" s="79"/>
-      <c r="E40" s="82"/>
-      <c r="F40" s="83"/>
+        <v>35.940000000000005</v>
+      </c>
+      <c r="D40" s="98"/>
+      <c r="E40" s="101"/>
+      <c r="F40" s="102"/>
       <c r="G40" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H40" s="42"/>
+      <c r="H40" s="41"/>
     </row>
     <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="37"/>
-      <c r="B41" s="38"/>
-      <c r="C41" s="78"/>
-      <c r="D41" s="79"/>
-      <c r="E41" s="80"/>
-      <c r="F41" s="81"/>
+      <c r="A41" s="36"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="97"/>
+      <c r="D41" s="98"/>
+      <c r="E41" s="99"/>
+      <c r="F41" s="100"/>
       <c r="G41" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H41" s="43">
+      <c r="H41" s="42">
         <f>IF(H39="",((SUM(H19:H37)))+H40,((SUM(H19:H37))*(1-H39))+H40)</f>
-        <v>33.99</v>
+        <v>29.950000000000003</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="37"/>
-      <c r="B42" s="38"/>
-      <c r="C42" s="78"/>
-      <c r="D42" s="79"/>
-      <c r="E42" s="80"/>
-      <c r="F42" s="81"/>
+      <c r="A42" s="36"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="97"/>
+      <c r="D42" s="98"/>
+      <c r="E42" s="99"/>
+      <c r="F42" s="100"/>
       <c r="G42" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H42" s="44">
+      <c r="H42" s="43">
         <f>ROUND(H41*0.2,2)</f>
-        <v>6.8</v>
+        <v>5.99</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="37"/>
-      <c r="B43" s="38"/>
-      <c r="C43" s="76"/>
-      <c r="D43" s="77"/>
-      <c r="E43" s="80"/>
-      <c r="F43" s="81"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="95"/>
+      <c r="D43" s="96"/>
+      <c r="E43" s="99"/>
+      <c r="F43" s="100"/>
       <c r="G43" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H43" s="40">
+      <c r="H43" s="39">
         <f>H41+H42</f>
-        <v>40.79</v>
+        <v>35.940000000000005</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="62" t="s">
+      <c r="A44" s="119" t="s">
         <v>23</v>
       </c>
-      <c r="B44" s="65">
+      <c r="B44" s="122">
         <f ca="1">TODAY()</f>
-        <v>43046</v>
-      </c>
-      <c r="C44" s="45" t="s">
+        <v>43129</v>
+      </c>
+      <c r="C44" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="D44" s="46"/>
-      <c r="E44" s="71" t="s">
+      <c r="D44" s="45"/>
+      <c r="E44" s="128" t="s">
+        <v>36</v>
+      </c>
+      <c r="F44" s="129"/>
+      <c r="G44" s="129"/>
+      <c r="H44" s="130"/>
+    </row>
+    <row r="45" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="120"/>
+      <c r="B45" s="123"/>
+      <c r="C45" s="125" t="s">
+        <v>34</v>
+      </c>
+      <c r="D45" s="126"/>
+      <c r="E45" s="127">
+        <v>7426192745</v>
+      </c>
+      <c r="F45" s="115"/>
+      <c r="G45" s="115"/>
+      <c r="H45" s="116"/>
+    </row>
+    <row r="46" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="120"/>
+      <c r="B46" s="123"/>
+      <c r="C46" s="125" t="s">
+        <v>33</v>
+      </c>
+      <c r="D46" s="126"/>
+      <c r="E46" s="114" t="s">
         <v>37</v>
       </c>
-      <c r="F44" s="72"/>
-      <c r="G44" s="72"/>
-      <c r="H44" s="73"/>
-    </row>
-    <row r="45" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="63"/>
-      <c r="B45" s="66"/>
-      <c r="C45" s="68" t="s">
-        <v>34</v>
-      </c>
-      <c r="D45" s="69"/>
-      <c r="E45" s="70">
-        <v>7426192745</v>
-      </c>
-      <c r="F45" s="57"/>
-      <c r="G45" s="57"/>
-      <c r="H45" s="58"/>
-    </row>
-    <row r="46" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="63"/>
-      <c r="B46" s="66"/>
-      <c r="C46" s="68" t="s">
-        <v>33</v>
-      </c>
-      <c r="D46" s="69"/>
-      <c r="E46" s="56" t="s">
-        <v>38</v>
-      </c>
-      <c r="F46" s="57"/>
-      <c r="G46" s="57"/>
-      <c r="H46" s="58"/>
+      <c r="F46" s="115"/>
+      <c r="G46" s="115"/>
+      <c r="H46" s="116"/>
     </row>
     <row r="47" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="64"/>
-      <c r="B47" s="67"/>
-      <c r="C47" s="47" t="s">
+      <c r="A47" s="121"/>
+      <c r="B47" s="124"/>
+      <c r="C47" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="48"/>
-      <c r="E47" s="59"/>
-      <c r="F47" s="60"/>
-      <c r="G47" s="60"/>
-      <c r="H47" s="61"/>
+      <c r="D47" s="47"/>
+      <c r="E47" s="137" t="s">
+        <v>41</v>
+      </c>
+      <c r="F47" s="117"/>
+      <c r="G47" s="117"/>
+      <c r="H47" s="118"/>
     </row>
     <row r="48" spans="1:8" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="105" t="s">
+      <c r="A48" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="B48" s="106"/>
-      <c r="C48" s="106"/>
-      <c r="D48" s="106"/>
-      <c r="E48" s="107"/>
-      <c r="F48" s="107"/>
-      <c r="G48" s="107"/>
-      <c r="H48" s="108"/>
+      <c r="B48" s="85"/>
+      <c r="C48" s="85"/>
+      <c r="D48" s="85"/>
+      <c r="E48" s="86"/>
+      <c r="F48" s="86"/>
+      <c r="G48" s="86"/>
+      <c r="H48" s="87"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="102"/>
-      <c r="B49" s="103"/>
-      <c r="C49" s="103"/>
-      <c r="D49" s="103"/>
-      <c r="E49" s="103"/>
-      <c r="F49" s="103"/>
-      <c r="G49" s="103"/>
-      <c r="H49" s="104"/>
+      <c r="A49" s="81"/>
+      <c r="B49" s="82"/>
+      <c r="C49" s="82"/>
+      <c r="D49" s="82"/>
+      <c r="E49" s="82"/>
+      <c r="F49" s="82"/>
+      <c r="G49" s="82"/>
+      <c r="H49" s="83"/>
     </row>
     <row r="50" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="102" t="s">
+      <c r="A50" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="B50" s="103"/>
-      <c r="C50" s="103"/>
-      <c r="D50" s="103"/>
-      <c r="E50" s="103"/>
-      <c r="F50" s="103"/>
-      <c r="G50" s="103"/>
-      <c r="H50" s="104"/>
+      <c r="B50" s="82"/>
+      <c r="C50" s="82"/>
+      <c r="D50" s="82"/>
+      <c r="E50" s="82"/>
+      <c r="F50" s="82"/>
+      <c r="G50" s="82"/>
+      <c r="H50" s="83"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="102"/>
-      <c r="B51" s="103"/>
-      <c r="C51" s="103"/>
-      <c r="D51" s="103"/>
-      <c r="E51" s="103"/>
-      <c r="F51" s="103"/>
-      <c r="G51" s="103"/>
-      <c r="H51" s="104"/>
+      <c r="A51" s="81"/>
+      <c r="B51" s="82"/>
+      <c r="C51" s="82"/>
+      <c r="D51" s="82"/>
+      <c r="E51" s="82"/>
+      <c r="F51" s="82"/>
+      <c r="G51" s="82"/>
+      <c r="H51" s="83"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="102"/>
-      <c r="B52" s="103"/>
-      <c r="C52" s="103"/>
-      <c r="D52" s="103"/>
-      <c r="E52" s="103"/>
-      <c r="F52" s="103"/>
-      <c r="G52" s="103"/>
-      <c r="H52" s="104"/>
+      <c r="A52" s="81"/>
+      <c r="B52" s="82"/>
+      <c r="C52" s="82"/>
+      <c r="D52" s="82"/>
+      <c r="E52" s="82"/>
+      <c r="F52" s="82"/>
+      <c r="G52" s="82"/>
+      <c r="H52" s="83"/>
     </row>
     <row r="53" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="102" t="s">
+      <c r="A53" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="B53" s="103"/>
-      <c r="C53" s="103"/>
-      <c r="D53" s="103"/>
-      <c r="E53" s="103"/>
-      <c r="F53" s="103"/>
-      <c r="G53" s="103"/>
-      <c r="H53" s="104"/>
+      <c r="B53" s="82"/>
+      <c r="C53" s="82"/>
+      <c r="D53" s="82"/>
+      <c r="E53" s="82"/>
+      <c r="F53" s="82"/>
+      <c r="G53" s="82"/>
+      <c r="H53" s="83"/>
     </row>
     <row r="54" spans="1:8" s="20" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="13" t="s">
@@ -3001,6 +3095,54 @@
     <protectedRange sqref="B19:E37" name="Description"/>
   </protectedRanges>
   <mergeCells count="64">
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="E46:H46"/>
+    <mergeCell ref="E47:H47"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E45:H45"/>
+    <mergeCell ref="E44:H44"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A52:H52"/>
+    <mergeCell ref="A53:H53"/>
+    <mergeCell ref="A48:H48"/>
+    <mergeCell ref="A49:H49"/>
+    <mergeCell ref="A50:H50"/>
+    <mergeCell ref="A51:H51"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="A17:D17"/>
@@ -3017,54 +3159,6 @@
     <mergeCell ref="C14:H14"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A52:H52"/>
-    <mergeCell ref="A53:H53"/>
-    <mergeCell ref="A48:H48"/>
-    <mergeCell ref="A49:H49"/>
-    <mergeCell ref="A50:H50"/>
-    <mergeCell ref="A51:H51"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="E46:H46"/>
-    <mergeCell ref="E47:H47"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E45:H45"/>
-    <mergeCell ref="E44:H44"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A33:D33"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>